<commit_message>
editing geneSearch for both common and rare inversion breakpoints
</commit_message>
<xml_diff>
--- a/Breakpoints.xlsx
+++ b/Breakpoints.xlsx
@@ -567,7 +567,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,26 +600,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -637,24 +617,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X58"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9387755102041"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,120 +2698,112 @@
       </c>
       <c r="J52" s="2"/>
     </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
+      <c r="A54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>8855599</v>
+      </c>
+      <c r="C54" s="6" t="n">
+        <v>8855976</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>-377</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="9" t="n">
-        <v>8855599</v>
-      </c>
-      <c r="C55" s="10" t="n">
-        <v>8855976</v>
-      </c>
-      <c r="D55" s="9" t="n">
-        <v>-377</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G55" s="9" t="s">
+      <c r="B55" s="3" t="n">
+        <v>17749316</v>
+      </c>
+      <c r="C55" s="6" t="n">
+        <v>17749303</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" s="9" t="n">
-        <v>17749316</v>
-      </c>
-      <c r="C56" s="10" t="n">
-        <v>17749303</v>
-      </c>
-      <c r="D56" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B57" s="10" t="n">
+      <c r="B56" s="6" t="n">
         <v>14591413</v>
       </c>
-      <c r="C57" s="10" t="n">
+      <c r="C56" s="6" t="n">
         <v>14590368</v>
       </c>
-      <c r="D57" s="9" t="n">
+      <c r="D56" s="3" t="n">
         <v>1045</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E56" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F56" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="12" t="s">
+      <c r="H56" s="2"/>
+      <c r="I56" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="10" t="n">
+      <c r="B57" s="6" t="n">
         <v>18774476</v>
       </c>
-      <c r="C58" s="10" t="n">
+      <c r="C57" s="6" t="n">
         <v>18774480</v>
       </c>
-      <c r="D58" s="9" t="n">
+      <c r="D57" s="3" t="n">
         <v>-4</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="G57" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
able to parse common inversions now in addition to rare
</commit_message>
<xml_diff>
--- a/Breakpoints.xlsx
+++ b/Breakpoints.xlsx
@@ -619,14 +619,13 @@
   </sheetPr>
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9387755102041"/>

</xml_diff>